<commit_message>
more artillery; cloud batch file
</commit_message>
<xml_diff>
--- a/artilleryScenarioCalcs.xlsx
+++ b/artilleryScenarioCalcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\performance_testing\artillery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E9C914-AAED-4498-A810-2CC0148E540C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967DE9FF-7FE6-459E-B877-5502D0A5A93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FC907127-9A7B-43B0-A1F5-421D8C823328}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t xml:space="preserve">Phase </t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t xml:space="preserve">VU ramped over all of the ramp+steady periods then 0; requests rose to a peak 175/sec then dropped to ~ 40/sec for </t>
+  </si>
+  <si>
+    <t>ACTUAL VU created</t>
+  </si>
+  <si>
+    <t>rampup as expected</t>
+  </si>
+  <si>
+    <t>asciiArt_2024-05-23_run01</t>
+  </si>
+  <si>
+    <t>PW (Playwright) run01</t>
   </si>
 </sst>
 </file>
@@ -505,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF768F28-D397-4E2D-B45F-A1611CCFC3EB}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,11 +535,11 @@
     <col min="8" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="4"/>
-    <col min="16" max="16" width="38.28515625" style="1" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="4"/>
+    <col min="17" max="17" width="38.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -567,17 +579,20 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -619,7 +634,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -661,7 +676,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -700,21 +715,21 @@
         <f>L5*10</f>
         <v>2175</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>181</v>
       </c>
-      <c r="O5" s="5">
+      <c r="P5" s="5">
         <f>(26886-26183)/26886</f>
         <v>2.6147437327977387E-2</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -758,17 +773,17 @@
         <f>L7*10</f>
         <v>175</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>18</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -779,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -825,7 +840,7 @@
         <v>37.220843672456574</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -834,6 +849,68 @@
       </c>
       <c r="D11">
         <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <f>AVERAGE(C13,D13)*E13</f>
+        <v>300</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>20</v>
+      </c>
+      <c r="K13">
+        <f>(G13*H13+I13)*J13</f>
+        <v>240</v>
+      </c>
+      <c r="L13" s="4">
+        <f>(F13*G13*J13)/K13</f>
+        <v>75</v>
+      </c>
+      <c r="M13" s="4">
+        <f>L13*10</f>
+        <v>750</v>
+      </c>
+      <c r="N13" s="4">
+        <v>300</v>
+      </c>
+      <c r="O13">
+        <v>750</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>